<commit_message>
Pre Phase 8 RPC migration
</commit_message>
<xml_diff>
--- a/opswork/AffiliateCC.xlsx
+++ b/opswork/AffiliateCC.xlsx
@@ -10,6 +10,15 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Meta-Category Mapping" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Meta-Category Summary" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Affiliate Matrix" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Engagement Driver Mapping" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Engagement Driver Summary" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Hook Strategy Affiliate Matrix" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Hook Strategy Mapping" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Hook Strategy Summary" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Hook Strategy Matrix" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CTA Strategy Mapping" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CTA Strategy Summary" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CTA Strategy Matrix" sheetId="12" state="visible" r:id="rId12"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -19,7 +28,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -30,13 +39,59 @@
     <font>
       <b val="1"/>
     </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="002E86AB"/>
+        <bgColor rgb="002E86AB"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E74C3C"/>
+        <bgColor rgb="00E74C3C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="003498DB"/>
+        <bgColor rgb="003498DB"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0027AE60"/>
+        <bgColor rgb="0027AE60"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F39C12"/>
+        <bgColor rgb="00F39C12"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="009B59B6"/>
+        <bgColor rgb="009B59B6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="001ABC9C"/>
+        <bgColor rgb="001ABC9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -57,10 +112,43 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -677,12 +765,6 @@
         </is>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="inlineStr"/>
-      <c r="B12" t="inlineStr"/>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
-    </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
@@ -815,12 +897,6 @@
         </is>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" t="inlineStr"/>
-      <c r="B19" t="inlineStr"/>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr"/>
-    </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
@@ -953,12 +1029,6 @@
         </is>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" t="inlineStr"/>
-      <c r="B26" t="inlineStr"/>
-      <c r="C26" t="inlineStr"/>
-      <c r="D26" t="inlineStr"/>
-    </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
@@ -1110,6 +1180,1142 @@
       <c r="D33" t="inlineStr">
         <is>
           <t>Casual audience acknowledgment</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="18" customWidth="1" min="1" max="1"/>
+    <col width="28" customWidth="1" min="2" max="2"/>
+    <col width="18" customWidth="1" min="3" max="3"/>
+    <col width="10" customWidth="1" min="4" max="4"/>
+    <col width="45" customWidth="1" min="5" max="5"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Semantic Category</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Original CTA</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Affiliate</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Usage %</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="5" t="inlineStr">
+        <is>
+          <t>DIRECT LINK</t>
+        </is>
+      </c>
+      <c r="B2" s="4" t="inlineStr">
+        <is>
+          <t>Link Direction</t>
+        </is>
+      </c>
+      <c r="C2" s="4" t="inlineStr">
+        <is>
+          <t>@yainafashion</t>
+        </is>
+      </c>
+      <c r="D2" s="4" t="inlineStr">
+        <is>
+          <t>95%</t>
+        </is>
+      </c>
+      <c r="E2" s="4" t="inlineStr">
+        <is>
+          <t>Dominant - directs to purchase link</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="inlineStr">
+        <is>
+          <t>DIRECT LINK</t>
+        </is>
+      </c>
+      <c r="B3" s="4" t="inlineStr">
+        <is>
+          <t>Link Direction CTA</t>
+        </is>
+      </c>
+      <c r="C3" s="4" t="inlineStr">
+        <is>
+          <t>@bomboncito127</t>
+        </is>
+      </c>
+      <c r="D3" s="4" t="inlineStr">
+        <is>
+          <t>92%</t>
+        </is>
+      </c>
+      <c r="E3" s="4" t="inlineStr">
+        <is>
+          <t>Dominant - directs to purchase link</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="5" t="inlineStr">
+        <is>
+          <t>DIRECT LINK</t>
+        </is>
+      </c>
+      <c r="B4" s="4" t="inlineStr">
+        <is>
+          <t>Product CTA With Platform</t>
+        </is>
+      </c>
+      <c r="C4" s="4" t="inlineStr">
+        <is>
+          <t>@ayunonutricion</t>
+        </is>
+      </c>
+      <c r="D4" s="4" t="inlineStr">
+        <is>
+          <t>34%</t>
+        </is>
+      </c>
+      <c r="E4" s="4" t="inlineStr">
+        <is>
+          <t>Product mention with platform direction</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="5" t="inlineStr">
+        <is>
+          <t>DIRECT LINK</t>
+        </is>
+      </c>
+      <c r="B5" s="4" t="inlineStr">
+        <is>
+          <t>Direct Link CTA</t>
+        </is>
+      </c>
+      <c r="C5" s="4" t="inlineStr">
+        <is>
+          <t>@shopbyjake</t>
+        </is>
+      </c>
+      <c r="D5" s="4" t="inlineStr">
+        <is>
+          <t>15%</t>
+        </is>
+      </c>
+      <c r="E5" s="4" t="inlineStr">
+        <is>
+          <t>Secondary - direct link</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="5" t="inlineStr">
+        <is>
+          <t>DIRECT LINK</t>
+        </is>
+      </c>
+      <c r="B6" s="4" t="inlineStr">
+        <is>
+          <t>Link Direction</t>
+        </is>
+      </c>
+      <c r="C6" s="4" t="inlineStr">
+        <is>
+          <t>@daisycabral_</t>
+        </is>
+      </c>
+      <c r="D6" s="4" t="inlineStr">
+        <is>
+          <t>15%</t>
+        </is>
+      </c>
+      <c r="E6" s="4" t="inlineStr">
+        <is>
+          <t>Secondary - directs to link</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="inlineStr">
+        <is>
+          <t>URGENCY/SCARCITY</t>
+        </is>
+      </c>
+      <c r="B7" s="4" t="inlineStr">
+        <is>
+          <t>Urgent CTA</t>
+        </is>
+      </c>
+      <c r="C7" s="4" t="inlineStr">
+        <is>
+          <t>@realkalimuscle</t>
+        </is>
+      </c>
+      <c r="D7" s="4" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="E7" s="4" t="inlineStr">
+        <is>
+          <t>Dominant - pure urgency</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="inlineStr">
+        <is>
+          <t>URGENCY/SCARCITY</t>
+        </is>
+      </c>
+      <c r="B8" s="4" t="inlineStr">
+        <is>
+          <t>Urgency Scarcity CTA</t>
+        </is>
+      </c>
+      <c r="C8" s="4" t="inlineStr">
+        <is>
+          <t>@realmrchicago</t>
+        </is>
+      </c>
+      <c r="D8" s="4" t="inlineStr">
+        <is>
+          <t>85%</t>
+        </is>
+      </c>
+      <c r="E8" s="4" t="inlineStr">
+        <is>
+          <t>Dominant - scarcity messaging</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="inlineStr">
+        <is>
+          <t>URGENCY/SCARCITY</t>
+        </is>
+      </c>
+      <c r="B9" s="4" t="inlineStr">
+        <is>
+          <t>Scarcity Urgency Close</t>
+        </is>
+      </c>
+      <c r="C9" s="4" t="inlineStr">
+        <is>
+          <t>@shopbyjake</t>
+        </is>
+      </c>
+      <c r="D9" s="4" t="inlineStr">
+        <is>
+          <t>83%</t>
+        </is>
+      </c>
+      <c r="E9" s="4" t="inlineStr">
+        <is>
+          <t>Dominant - urgency close</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="7" t="inlineStr">
+        <is>
+          <t>ENGAGEMENT</t>
+        </is>
+      </c>
+      <c r="B10" s="4" t="inlineStr">
+        <is>
+          <t>Comment Prompt</t>
+        </is>
+      </c>
+      <c r="C10" s="4" t="inlineStr">
+        <is>
+          <t>@daisycabral_</t>
+        </is>
+      </c>
+      <c r="D10" s="4" t="inlineStr">
+        <is>
+          <t>28%</t>
+        </is>
+      </c>
+      <c r="E10" s="4" t="inlineStr">
+        <is>
+          <t>Asks for comments</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="7" t="inlineStr">
+        <is>
+          <t>ENGAGEMENT</t>
+        </is>
+      </c>
+      <c r="B11" s="4" t="inlineStr">
+        <is>
+          <t>Engagement Challenge</t>
+        </is>
+      </c>
+      <c r="C11" s="4" t="inlineStr">
+        <is>
+          <t>@realmrchicago</t>
+        </is>
+      </c>
+      <c r="D11" s="4" t="inlineStr">
+        <is>
+          <t>15%</t>
+        </is>
+      </c>
+      <c r="E11" s="4" t="inlineStr">
+        <is>
+          <t>Challenges viewers to engage</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="7" t="inlineStr">
+        <is>
+          <t>ENGAGEMENT</t>
+        </is>
+      </c>
+      <c r="B12" s="4" t="inlineStr">
+        <is>
+          <t>Engagement Request</t>
+        </is>
+      </c>
+      <c r="C12" s="4" t="inlineStr">
+        <is>
+          <t>@ayunonutricion</t>
+        </is>
+      </c>
+      <c r="D12" s="4" t="inlineStr">
+        <is>
+          <t>15%</t>
+        </is>
+      </c>
+      <c r="E12" s="4" t="inlineStr">
+        <is>
+          <t>Requests engagement</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="7" t="inlineStr">
+        <is>
+          <t>ENGAGEMENT</t>
+        </is>
+      </c>
+      <c r="B13" s="4" t="inlineStr">
+        <is>
+          <t>Dare Challenge Close</t>
+        </is>
+      </c>
+      <c r="C13" s="4" t="inlineStr">
+        <is>
+          <t>@shopbyjake</t>
+        </is>
+      </c>
+      <c r="D13" s="4" t="inlineStr">
+        <is>
+          <t>3%</t>
+        </is>
+      </c>
+      <c r="E13" s="4" t="inlineStr">
+        <is>
+          <t>Challenges viewers</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="6" t="inlineStr">
+        <is>
+          <t>SOFT/GRATITUDE</t>
+        </is>
+      </c>
+      <c r="B14" s="4" t="inlineStr">
+        <is>
+          <t>Encouragement To Act</t>
+        </is>
+      </c>
+      <c r="C14" s="4" t="inlineStr">
+        <is>
+          <t>@ayunonutricion</t>
+        </is>
+      </c>
+      <c r="D14" s="4" t="inlineStr">
+        <is>
+          <t>34%</t>
+        </is>
+      </c>
+      <c r="E14" s="4" t="inlineStr">
+        <is>
+          <t>Soft encouragement</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="6" t="inlineStr">
+        <is>
+          <t>SOFT/GRATITUDE</t>
+        </is>
+      </c>
+      <c r="B15" s="4" t="inlineStr">
+        <is>
+          <t>Gratitude Closing</t>
+        </is>
+      </c>
+      <c r="C15" s="4" t="inlineStr">
+        <is>
+          <t>@ayunonutricion</t>
+        </is>
+      </c>
+      <c r="D15" s="4" t="inlineStr">
+        <is>
+          <t>17%</t>
+        </is>
+      </c>
+      <c r="E15" s="4" t="inlineStr">
+        <is>
+          <t>Thanks viewers</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="6" t="inlineStr">
+        <is>
+          <t>SOFT/GRATITUDE</t>
+        </is>
+      </c>
+      <c r="B16" s="4" t="inlineStr">
+        <is>
+          <t>Benefit Reinforcement</t>
+        </is>
+      </c>
+      <c r="C16" s="4" t="inlineStr">
+        <is>
+          <t>@bomboncito127</t>
+        </is>
+      </c>
+      <c r="D16" s="4" t="inlineStr">
+        <is>
+          <t>7%</t>
+        </is>
+      </c>
+      <c r="E16" s="4" t="inlineStr">
+        <is>
+          <t>Reinforces benefits softly</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="6" t="inlineStr">
+        <is>
+          <t>SOFT/GRATITUDE</t>
+        </is>
+      </c>
+      <c r="B17" s="4" t="inlineStr">
+        <is>
+          <t>Gratitude Closing</t>
+        </is>
+      </c>
+      <c r="C17" s="4" t="inlineStr">
+        <is>
+          <t>@yainafashion</t>
+        </is>
+      </c>
+      <c r="D17" s="4" t="inlineStr">
+        <is>
+          <t>3%</t>
+        </is>
+      </c>
+      <c r="E17" s="4" t="inlineStr">
+        <is>
+          <t>Thanks viewers</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="6" t="inlineStr">
+        <is>
+          <t>SOFT/GRATITUDE</t>
+        </is>
+      </c>
+      <c r="B18" s="4" t="inlineStr">
+        <is>
+          <t>Gratitude Close</t>
+        </is>
+      </c>
+      <c r="C18" s="4" t="inlineStr">
+        <is>
+          <t>@daisycabral_</t>
+        </is>
+      </c>
+      <c r="D18" s="4" t="inlineStr">
+        <is>
+          <t>2%</t>
+        </is>
+      </c>
+      <c r="E18" s="4" t="inlineStr">
+        <is>
+          <t>Thanks viewers</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="6" t="inlineStr">
+        <is>
+          <t>SOFT/GRATITUDE</t>
+        </is>
+      </c>
+      <c r="B19" s="4" t="inlineStr">
+        <is>
+          <t>Simple Goodbye</t>
+        </is>
+      </c>
+      <c r="C19" s="4" t="inlineStr">
+        <is>
+          <t>@yainafashion</t>
+        </is>
+      </c>
+      <c r="D19" s="4" t="inlineStr">
+        <is>
+          <t>2%</t>
+        </is>
+      </c>
+      <c r="E19" s="4" t="inlineStr">
+        <is>
+          <t>Simple goodbye</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="8" t="inlineStr">
+        <is>
+          <t>LIVE INVITATION</t>
+        </is>
+      </c>
+      <c r="B20" s="4" t="inlineStr">
+        <is>
+          <t>Live Invitation</t>
+        </is>
+      </c>
+      <c r="C20" s="4" t="inlineStr">
+        <is>
+          <t>@daisycabral_</t>
+        </is>
+      </c>
+      <c r="D20" s="4" t="inlineStr">
+        <is>
+          <t>53%</t>
+        </is>
+      </c>
+      <c r="E20" s="4" t="inlineStr">
+        <is>
+          <t>OUTLIER - Livestream-specific, signature style</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="8" t="inlineStr">
+        <is>
+          <t>LIVE INVITATION</t>
+        </is>
+      </c>
+      <c r="B21" s="4" t="inlineStr">
+        <is>
+          <t>Inclusive Invitation</t>
+        </is>
+      </c>
+      <c r="C21" s="4" t="inlineStr">
+        <is>
+          <t>@bomboncito127</t>
+        </is>
+      </c>
+      <c r="D21" s="4" t="inlineStr">
+        <is>
+          <t>1%</t>
+        </is>
+      </c>
+      <c r="E21" s="4" t="inlineStr">
+        <is>
+          <t>Trace level - general invitation</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="18" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="40" customWidth="1" min="3" max="3"/>
+    <col width="18" customWidth="1" min="4" max="4"/>
+    <col width="8" customWidth="1" min="5" max="5"/>
+    <col width="50" customWidth="1" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Semantic Category</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Reach</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Affiliates Using</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Top Performer</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Top %</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Definition</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="5" t="inlineStr">
+        <is>
+          <t>DIRECT LINK</t>
+        </is>
+      </c>
+      <c r="B2" s="10" t="inlineStr">
+        <is>
+          <t>5/7 (71%)</t>
+        </is>
+      </c>
+      <c r="C2" s="4" t="inlineStr">
+        <is>
+          <t>yaina, bomboncito, ayuno, shopbyjake, daisy</t>
+        </is>
+      </c>
+      <c r="D2" s="4" t="inlineStr">
+        <is>
+          <t>@yainafashion</t>
+        </is>
+      </c>
+      <c r="E2" s="4" t="inlineStr">
+        <is>
+          <t>95%</t>
+        </is>
+      </c>
+      <c r="F2" s="4" t="inlineStr">
+        <is>
+          <t>Closes by directing viewers to purchase link</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>URGENCY/SCARCITY</t>
+        </is>
+      </c>
+      <c r="B3" s="10" t="inlineStr">
+        <is>
+          <t>3/7 (43%)</t>
+        </is>
+      </c>
+      <c r="C3" s="4" t="inlineStr">
+        <is>
+          <t>kalimuscle, mrchicago, shopbyjake</t>
+        </is>
+      </c>
+      <c r="D3" s="4" t="inlineStr">
+        <is>
+          <t>@realkalimuscle</t>
+        </is>
+      </c>
+      <c r="E3" s="4" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="F3" s="4" t="inlineStr">
+        <is>
+          <t>Closes with time pressure or scarcity</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="7" t="inlineStr">
+        <is>
+          <t>ENGAGEMENT</t>
+        </is>
+      </c>
+      <c r="B4" s="10" t="inlineStr">
+        <is>
+          <t>4/7 (57%)</t>
+        </is>
+      </c>
+      <c r="C4" s="4" t="inlineStr">
+        <is>
+          <t>daisy, mrchicago, ayuno, shopbyjake</t>
+        </is>
+      </c>
+      <c r="D4" s="4" t="inlineStr">
+        <is>
+          <t>@daisycabral_</t>
+        </is>
+      </c>
+      <c r="E4" s="4" t="inlineStr">
+        <is>
+          <t>28%</t>
+        </is>
+      </c>
+      <c r="F4" s="4" t="inlineStr">
+        <is>
+          <t>Closes by asking for comments or engagement</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="6" t="inlineStr">
+        <is>
+          <t>SOFT/GRATITUDE</t>
+        </is>
+      </c>
+      <c r="B5" s="10" t="inlineStr">
+        <is>
+          <t>3/7 (43%)</t>
+        </is>
+      </c>
+      <c r="C5" s="4" t="inlineStr">
+        <is>
+          <t>ayuno, bomboncito, yaina, daisy</t>
+        </is>
+      </c>
+      <c r="D5" s="4" t="inlineStr">
+        <is>
+          <t>@ayunonutricion</t>
+        </is>
+      </c>
+      <c r="E5" s="4" t="inlineStr">
+        <is>
+          <t>34%</t>
+        </is>
+      </c>
+      <c r="F5" s="4" t="inlineStr">
+        <is>
+          <t>Closes with gratitude, encouragement, or soft goodbye</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="8" t="inlineStr">
+        <is>
+          <t>LIVE INVITATION</t>
+        </is>
+      </c>
+      <c r="B6" s="10" t="inlineStr">
+        <is>
+          <t>1/7 (14%)</t>
+        </is>
+      </c>
+      <c r="C6" s="4" t="inlineStr">
+        <is>
+          <t>daisy (OUTLIER)</t>
+        </is>
+      </c>
+      <c r="D6" s="4" t="inlineStr">
+        <is>
+          <t>@daisycabral_</t>
+        </is>
+      </c>
+      <c r="E6" s="4" t="inlineStr">
+        <is>
+          <t>53%</t>
+        </is>
+      </c>
+      <c r="F6" s="4" t="inlineStr">
+        <is>
+          <t>OUTLIER - Invites viewers to join livestream</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="18" customWidth="1" min="1" max="1"/>
+    <col width="16" customWidth="1" min="2" max="2"/>
+    <col width="16" customWidth="1" min="3" max="3"/>
+    <col width="16" customWidth="1" min="4" max="4"/>
+    <col width="16" customWidth="1" min="5" max="5"/>
+    <col width="16" customWidth="1" min="6" max="6"/>
+    <col width="24" customWidth="1" min="7" max="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="30" customHeight="1">
+      <c r="A1" s="11" t="inlineStr">
+        <is>
+          <t>Affiliate</t>
+        </is>
+      </c>
+      <c r="B1" s="11" t="inlineStr">
+        <is>
+          <t>DIRECT LINK</t>
+        </is>
+      </c>
+      <c r="C1" s="11" t="inlineStr">
+        <is>
+          <t>URGENCY/SCARCITY</t>
+        </is>
+      </c>
+      <c r="D1" s="11" t="inlineStr">
+        <is>
+          <t>ENGAGEMENT</t>
+        </is>
+      </c>
+      <c r="E1" s="11" t="inlineStr">
+        <is>
+          <t>SOFT/GRATITUDE</t>
+        </is>
+      </c>
+      <c r="F1" s="11" t="inlineStr">
+        <is>
+          <t>LIVE INVITATION</t>
+        </is>
+      </c>
+      <c r="G1" s="11" t="inlineStr">
+        <is>
+          <t>Dominant CTA</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="10" t="inlineStr">
+        <is>
+          <t>@daisycabral_</t>
+        </is>
+      </c>
+      <c r="B2" s="10" t="inlineStr">
+        <is>
+          <t>15%</t>
+        </is>
+      </c>
+      <c r="C2" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D2" s="12" t="inlineStr">
+        <is>
+          <t>28%</t>
+        </is>
+      </c>
+      <c r="E2" s="10" t="inlineStr">
+        <is>
+          <t>2%</t>
+        </is>
+      </c>
+      <c r="F2" s="6" t="inlineStr">
+        <is>
+          <t>53%</t>
+        </is>
+      </c>
+      <c r="G2" s="10" t="inlineStr">
+        <is>
+          <t>LIVE INVITATION (53%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="10" t="inlineStr">
+        <is>
+          <t>@realkalimuscle</t>
+        </is>
+      </c>
+      <c r="B3" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C3" s="6" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="D3" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E3" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F3" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G3" s="10" t="inlineStr">
+        <is>
+          <t>URGENCY (100%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="10" t="inlineStr">
+        <is>
+          <t>@shopbyjake</t>
+        </is>
+      </c>
+      <c r="B4" s="10" t="inlineStr">
+        <is>
+          <t>15%</t>
+        </is>
+      </c>
+      <c r="C4" s="6" t="inlineStr">
+        <is>
+          <t>83%</t>
+        </is>
+      </c>
+      <c r="D4" s="10" t="inlineStr">
+        <is>
+          <t>3%</t>
+        </is>
+      </c>
+      <c r="E4" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F4" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G4" s="10" t="inlineStr">
+        <is>
+          <t>URGENCY (83%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="10" t="inlineStr">
+        <is>
+          <t>@ayunonutricion</t>
+        </is>
+      </c>
+      <c r="B5" s="12" t="inlineStr">
+        <is>
+          <t>34%</t>
+        </is>
+      </c>
+      <c r="C5" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D5" s="10" t="inlineStr">
+        <is>
+          <t>15%</t>
+        </is>
+      </c>
+      <c r="E5" s="6" t="inlineStr">
+        <is>
+          <t>51%</t>
+        </is>
+      </c>
+      <c r="F5" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G5" s="10" t="inlineStr">
+        <is>
+          <t>SOFT/GRATITUDE (51%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="10" t="inlineStr">
+        <is>
+          <t>@yainafashion</t>
+        </is>
+      </c>
+      <c r="B6" s="6" t="inlineStr">
+        <is>
+          <t>95%</t>
+        </is>
+      </c>
+      <c r="C6" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D6" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E6" s="10" t="inlineStr">
+        <is>
+          <t>5%</t>
+        </is>
+      </c>
+      <c r="F6" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G6" s="10" t="inlineStr">
+        <is>
+          <t>DIRECT LINK (95%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="10" t="inlineStr">
+        <is>
+          <t>@bomboncito127</t>
+        </is>
+      </c>
+      <c r="B7" s="6" t="inlineStr">
+        <is>
+          <t>92%</t>
+        </is>
+      </c>
+      <c r="C7" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D7" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E7" s="10" t="inlineStr">
+        <is>
+          <t>7%</t>
+        </is>
+      </c>
+      <c r="F7" s="10" t="inlineStr">
+        <is>
+          <t>1%</t>
+        </is>
+      </c>
+      <c r="G7" s="10" t="inlineStr">
+        <is>
+          <t>DIRECT LINK (92%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="10" t="inlineStr">
+        <is>
+          <t>@realmrchicago</t>
+        </is>
+      </c>
+      <c r="B8" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C8" s="6" t="inlineStr">
+        <is>
+          <t>85%</t>
+        </is>
+      </c>
+      <c r="D8" s="10" t="inlineStr">
+        <is>
+          <t>15%</t>
+        </is>
+      </c>
+      <c r="E8" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F8" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G8" s="10" t="inlineStr">
+        <is>
+          <t>URGENCY (85%)</t>
         </is>
       </c>
     </row>
@@ -1270,6 +2476,1223 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>AFFILIATE</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>BRAND PROMOTED</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>🛒 PROMOTION</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>📦 SHOWCASE</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>📚 EDUCATION</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>🎭 PERSONAL BRAND</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>DOMINANT STRATEGY</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>@daisycabral_</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Bella All Natural</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>45%</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>26%</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>4%</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>24%</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>99%</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>PROMOTION (Livestream) 45%</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>@realkalimuscle</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Goli Nutrition</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>3%</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>27%</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>66%</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>3%</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>99%</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>EDUCATION-first (66%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>@realmrchicago</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Toplux</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>62%</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>38%</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>PROMOTION + PERSONAL BRAND</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>@yainafashion</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Physician's Choice</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>21%</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>79%</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>1%</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>101%</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>SHOWCASE-first (79%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>@bomboncito127</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Snap Supplements</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>58%</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>20%</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>22%</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>PROMOTION-first (58%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>@shopbyjake</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Micro Ingredients</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>52%</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>21%</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>23%</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>96%</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>PROMOTION (Comparison) 52%</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>@ayunonutricion</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Micro Ingredients</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>40%</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>9%</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>45%</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>5%</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>99%</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>EDUCATION + PROMOTION</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>META-CATEGORY</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>ORIGINAL DRIVER</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>AFFILIATE</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>PCT</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>SEMANTIC RATIONALE</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>PRODUCT DEMONSTRATION</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Product Demonstrations</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>@daisycabral_</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>36</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Showing product features on camera</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>PRODUCT DEMONSTRATION</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Real Time Demonstration</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>@realkalimuscle</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>53</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Demonstrating product in real-time</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>PRODUCT DEMONSTRATION</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Quality Demonstration</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>@yainafashion</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>90</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Showing product quality visually</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>PRODUCT DEMONSTRATION</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Showing Product Packaging</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>@ayunonutricion</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>25</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Displaying product packaging</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>PRODUCT DEMONSTRATION</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Showing On Camera</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>@bomboncito127</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>38</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Product visible on camera</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>PRODUCT DEMONSTRATION</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Close Up Shots</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>@yainafashion</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>72</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Close-up visual of product</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>PRODUCT DEMONSTRATION</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Multiple Color Showcase</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>@yainafashion</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>26</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Showing product variations</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>PRODUCT DEMONSTRATION</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Sizing Transparency</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>@yainafashion</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>28</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Showing fit/size details</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>TRANSFORMATION</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Before After Comparison</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>@realkalimuscle</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>63</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Showing transformation results</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>TRANSFORMATION</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Before After Reveal</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>@shopbyjake</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>53</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Revealing before/after</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>TRANSFORMATION</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Before After Mention</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>@bomboncito127</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>29</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Mentioning transformation</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>PERSONAL TESTIMONY</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Personal Testimony</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>@realkalimuscle</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>76</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>First-person experience</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>PERSONAL TESTIMONY</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Personal Testimony</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>@bomboncito127</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>64</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>First-person experience</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>PERSONAL TESTIMONY</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Real Testimonials</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>@shopbyjake</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>49</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Real user testimonials</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>PERSONAL TESTIMONY</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Age Milestone Wisdom</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>@realmrchicago</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>33</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Personal life wisdom</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>CREDIBILITY</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Price Comparison</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>@realkalimuscle</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>51</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Comparing value/price</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>CREDIBILITY</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Price Comparison</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>@shopbyjake</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>32</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Comparing value/price</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>CREDIBILITY</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Expert Citation</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>@shopbyjake</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>28</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Citing expertise</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>CREDIBILITY</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Explaining Scientific Mechanisms</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>@ayunonutricion</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>45</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Scientific explanations</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>URGENCY/SCARCITY</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Countdown To Live</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>@daisycabral_</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>28</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Live event countdown</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>URGENCY/SCARCITY</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Limited Time Offers</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>@daisycabral_</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>23</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Time-limited deals</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>URGENCY/SCARCITY</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Milestone Celebrations</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>@daisycabral_</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>25</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Achievement/milestone FOMO</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>URGENCY/SCARCITY</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Scarcity Urgency Messaging</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>@realmrchicago</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>67</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Scarcity pressure</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>DIRECT ENGAGEMENT</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Addressing Comments Directly</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>@ayunonutricion</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>17</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Responding to viewers</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>DIRECT ENGAGEMENT</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Direct Address Viewer</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>@bomboncito127</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>20</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Speaking directly to viewer</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>DIRECT ENGAGEMENT</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Direct Confrontation Tone</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>@realmrchicago</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>44</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Confrontational engagement</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>DIRECT ENGAGEMENT</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Shock Value Language</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>@realmrchicago</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>76</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Provocative engagement</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>META-CATEGORY</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t># ORIGINAL DRIVERS</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t># AFFILIATES USING</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>PSYCHOLOGICAL TRIGGER</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>PERSONAL TESTIMONY</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>4/7 (57%)</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Builds trust through first-person stories</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>TRANSFORMATION</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>3/7 (43%)</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Shows results are real with before/after</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>CREDIBILITY</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>4</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>3/7 (43%)</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Builds rational trust through expertise/value</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>DIRECT ENGAGEMENT</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>3/7 (43%)</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Creates connection through viewer interaction</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>URGENCY/SCARCITY</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2/7 (29%)</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Creates pressure to act now</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1281,37 +3704,37 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AFFILIATE</t>
+          <t>Affiliate</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>BRAND PROMOTED</t>
+          <t>DIRECT/PRODUCT</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>🛒 PROMOTION</t>
+          <t>PROBLEM/PAIN</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>📦 SHOWCASE</t>
+          <t>QUESTION</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>📚 EDUCATION</t>
+          <t>URGENCY/COMMAND</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>🎭 PERSONAL BRAND</t>
+          <t>PERSONAL/STORY</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>DOMINANT STRATEGY</t>
+          <t>Primary Hook Style</t>
         </is>
       </c>
     </row>
@@ -1323,32 +3746,32 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Bella All Natural</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>45%</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>26%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>2%</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>24%</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>PROMOTION (Livestream)</t>
+          <t>DIRECT/PRODUCT (Greeting-based)</t>
         </is>
       </c>
     </row>
@@ -1360,32 +3783,32 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Goli Nutrition</t>
+          <t>39%</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>62%</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>27%</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>66%</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>EDUCATION-first</t>
+          <t>PROBLEM/PAIN (Problem Declaration)</t>
         </is>
       </c>
     </row>
@@ -1397,32 +3820,32 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Micro Ingredients</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>52%</t>
+          <t>63%</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>21%</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>23%</t>
+          <t>2%</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>34%</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>PROMOTION (Comparison)</t>
+          <t>PROBLEM/PAIN (Negative Callout)</t>
         </is>
       </c>
     </row>
@@ -1434,32 +3857,32 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Micro Ingredients</t>
+          <t>54%</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>40%</t>
+          <t>14%</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>9%</t>
+          <t>13%</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>45%</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>5%</t>
+          <t>19%</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>EDUCATION + PROMOTION</t>
+          <t>DIRECT/PRODUCT (Presentation)</t>
         </is>
       </c>
     </row>
@@ -1471,22 +3894,22 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Physician's Choice</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>21%</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>79%</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -1496,7 +3919,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>SHOWCASE-first</t>
+          <t>DIRECT/PRODUCT (Demonstration)</t>
         </is>
       </c>
     </row>
@@ -1508,32 +3931,32 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Snap Supplements</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>58%</t>
+          <t>23%</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
+          <t>41%</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>15%</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
           <t>20%</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>22%</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>PROMOTION-first</t>
+          <t>QUESTION (Direct Question)</t>
         </is>
       </c>
     </row>
@@ -1545,32 +3968,1268 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Toplux</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
+          <t>11%</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>88%</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2%</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>URGENCY/COMMAND (Confrontation)</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="18" customWidth="1" min="1" max="1"/>
+    <col width="28" customWidth="1" min="2" max="2"/>
+    <col width="18" customWidth="1" min="3" max="3"/>
+    <col width="10" customWidth="1" min="4" max="4"/>
+    <col width="45" customWidth="1" min="5" max="5"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Semantic Category</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Original Hook</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Affiliate</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Usage %</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="inlineStr">
+        <is>
+          <t>PROBLEM/PAIN</t>
+        </is>
+      </c>
+      <c r="B2" s="4" t="inlineStr">
+        <is>
+          <t>Problem Declaration</t>
+        </is>
+      </c>
+      <c r="C2" s="4" t="inlineStr">
+        <is>
+          <t>@realkalimuscle</t>
+        </is>
+      </c>
+      <c r="D2" s="4" t="inlineStr">
+        <is>
+          <t>55%</t>
+        </is>
+      </c>
+      <c r="E2" s="4" t="inlineStr">
+        <is>
+          <t>Relatable problems (sugar cravings, weight)</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>PROBLEM/PAIN</t>
+        </is>
+      </c>
+      <c r="B3" s="4" t="inlineStr">
+        <is>
+          <t>Conditional Statement</t>
+        </is>
+      </c>
+      <c r="C3" s="4" t="inlineStr">
+        <is>
+          <t>@realkalimuscle</t>
+        </is>
+      </c>
+      <c r="D3" s="4" t="inlineStr">
+        <is>
+          <t>7%</t>
+        </is>
+      </c>
+      <c r="E3" s="4" t="inlineStr">
+        <is>
+          <t>If-statements targeting problems</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>PROBLEM/PAIN</t>
+        </is>
+      </c>
+      <c r="B4" s="4" t="inlineStr">
+        <is>
+          <t>Negative Product Callout</t>
+        </is>
+      </c>
+      <c r="C4" s="4" t="inlineStr">
+        <is>
+          <t>@shopbyjake</t>
+        </is>
+      </c>
+      <c r="D4" s="4" t="inlineStr">
+        <is>
+          <t>63%</t>
+        </is>
+      </c>
+      <c r="E4" s="4" t="inlineStr">
+        <is>
+          <t>Calling out product problems/scams</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>PROBLEM/PAIN</t>
+        </is>
+      </c>
+      <c r="B5" s="4" t="inlineStr">
+        <is>
+          <t>Problem Identification</t>
+        </is>
+      </c>
+      <c r="C5" s="4" t="inlineStr">
+        <is>
+          <t>@ayunonutricion</t>
+        </is>
+      </c>
+      <c r="D5" s="4" t="inlineStr">
+        <is>
+          <t>14%</t>
+        </is>
+      </c>
+      <c r="E5" s="4" t="inlineStr">
+        <is>
+          <t>Health problem/symptom identification</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="inlineStr">
+        <is>
+          <t>PROBLEM/PAIN</t>
+        </is>
+      </c>
+      <c r="B6" s="4" t="inlineStr">
+        <is>
+          <t>Problem Identification</t>
+        </is>
+      </c>
+      <c r="C6" s="4" t="inlineStr">
+        <is>
+          <t>@bomboncito127</t>
+        </is>
+      </c>
+      <c r="D6" s="4" t="inlineStr">
+        <is>
+          <t>23%</t>
+        </is>
+      </c>
+      <c r="E6" s="4" t="inlineStr">
+        <is>
+          <t>Relatable viewer problems</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="inlineStr">
+        <is>
+          <t>PROBLEM/PAIN</t>
+        </is>
+      </c>
+      <c r="B7" s="4" t="inlineStr">
+        <is>
+          <t>Symptom Checklist</t>
+        </is>
+      </c>
+      <c r="C7" s="4" t="inlineStr">
+        <is>
+          <t>@realmrchicago</t>
+        </is>
+      </c>
+      <c r="D7" s="4" t="inlineStr">
+        <is>
+          <t>11%</t>
+        </is>
+      </c>
+      <c r="E7" s="4" t="inlineStr">
+        <is>
+          <t>Relatable symptoms/conditions</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="5" t="inlineStr">
+        <is>
+          <t>PRODUCT-FIRST</t>
+        </is>
+      </c>
+      <c r="B8" s="4" t="inlineStr">
+        <is>
+          <t>Product Demonstration</t>
+        </is>
+      </c>
+      <c r="C8" s="4" t="inlineStr">
+        <is>
+          <t>@yainafashion</t>
+        </is>
+      </c>
+      <c r="D8" s="4" t="inlineStr">
+        <is>
+          <t>95%</t>
+        </is>
+      </c>
+      <c r="E8" s="4" t="inlineStr">
+        <is>
+          <t>Immediate product showing</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="5" t="inlineStr">
+        <is>
+          <t>PRODUCT-FIRST</t>
+        </is>
+      </c>
+      <c r="B9" s="4" t="inlineStr">
+        <is>
+          <t>Direct Presentation</t>
+        </is>
+      </c>
+      <c r="C9" s="4" t="inlineStr">
+        <is>
+          <t>@ayunonutricion</t>
+        </is>
+      </c>
+      <c r="D9" s="4" t="inlineStr">
+        <is>
+          <t>54%</t>
+        </is>
+      </c>
+      <c r="E9" s="4" t="inlineStr">
+        <is>
+          <t>Immediate product intro</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="5" t="inlineStr">
+        <is>
+          <t>PRODUCT-FIRST</t>
+        </is>
+      </c>
+      <c r="B10" s="4" t="inlineStr">
+        <is>
+          <t>Demonstration Opener</t>
+        </is>
+      </c>
+      <c r="C10" s="4" t="inlineStr">
+        <is>
+          <t>@realkalimuscle</t>
+        </is>
+      </c>
+      <c r="D10" s="4" t="inlineStr">
+        <is>
+          <t>27%</t>
+        </is>
+      </c>
+      <c r="E10" s="4" t="inlineStr">
+        <is>
+          <t>Product arrival/review setup</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="5" t="inlineStr">
+        <is>
+          <t>PRODUCT-FIRST</t>
+        </is>
+      </c>
+      <c r="B11" s="4" t="inlineStr">
+        <is>
+          <t>Attention Declaration</t>
+        </is>
+      </c>
+      <c r="C11" s="4" t="inlineStr">
+        <is>
+          <t>@daisycabral_</t>
+        </is>
+      </c>
+      <c r="D11" s="4" t="inlineStr">
+        <is>
+          <t>19%</t>
+        </is>
+      </c>
+      <c r="E11" s="4" t="inlineStr">
+        <is>
+          <t>Announcing intent to show/demo</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="6" t="inlineStr">
+        <is>
+          <t>PERSONAL/STORY</t>
+        </is>
+      </c>
+      <c r="B12" s="4" t="inlineStr">
+        <is>
+          <t>Personal Transformation Reveal</t>
+        </is>
+      </c>
+      <c r="C12" s="4" t="inlineStr">
+        <is>
+          <t>@shopbyjake</t>
+        </is>
+      </c>
+      <c r="D12" s="4" t="inlineStr">
+        <is>
+          <t>16%</t>
+        </is>
+      </c>
+      <c r="E12" s="4" t="inlineStr">
+        <is>
+          <t>Personal struggles/transformation</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="6" t="inlineStr">
+        <is>
+          <t>PERSONAL/STORY</t>
+        </is>
+      </c>
+      <c r="B13" s="4" t="inlineStr">
+        <is>
+          <t>Personal Declaration</t>
+        </is>
+      </c>
+      <c r="C13" s="4" t="inlineStr">
+        <is>
+          <t>@ayunonutricion</t>
+        </is>
+      </c>
+      <c r="D13" s="4" t="inlineStr">
+        <is>
+          <t>19%</t>
+        </is>
+      </c>
+      <c r="E13" s="4" t="inlineStr">
+        <is>
+          <t>Personal habits/routines</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="6" t="inlineStr">
+        <is>
+          <t>PERSONAL/STORY</t>
+        </is>
+      </c>
+      <c r="B14" s="4" t="inlineStr">
+        <is>
+          <t>Personal Story</t>
+        </is>
+      </c>
+      <c r="C14" s="4" t="inlineStr">
+        <is>
+          <t>@yainafashion</t>
+        </is>
+      </c>
+      <c r="D14" s="4" t="inlineStr">
+        <is>
+          <t>1%</t>
+        </is>
+      </c>
+      <c r="E14" s="4" t="inlineStr">
+        <is>
+          <t>Personal narrative</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="6" t="inlineStr">
+        <is>
+          <t>PERSONAL/STORY</t>
+        </is>
+      </c>
+      <c r="B15" s="4" t="inlineStr">
+        <is>
+          <t>Testimonial Opening</t>
+        </is>
+      </c>
+      <c r="C15" s="4" t="inlineStr">
+        <is>
+          <t>@bomboncito127</t>
+        </is>
+      </c>
+      <c r="D15" s="4" t="inlineStr">
+        <is>
+          <t>20%</t>
+        </is>
+      </c>
+      <c r="E15" s="4" t="inlineStr">
+        <is>
+          <t>Personal/family experience</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="7" t="inlineStr">
+        <is>
+          <t>QUESTION</t>
+        </is>
+      </c>
+      <c r="B16" s="4" t="inlineStr">
+        <is>
+          <t>Question Address</t>
+        </is>
+      </c>
+      <c r="C16" s="4" t="inlineStr">
+        <is>
+          <t>@daisycabral_</t>
+        </is>
+      </c>
+      <c r="D16" s="4" t="inlineStr">
+        <is>
+          <t>4%</t>
+        </is>
+      </c>
+      <c r="E16" s="4" t="inlineStr">
+        <is>
+          <t>Direct question to viewer</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="7" t="inlineStr">
+        <is>
+          <t>QUESTION</t>
+        </is>
+      </c>
+      <c r="B17" s="4" t="inlineStr">
+        <is>
+          <t>Direct Question</t>
+        </is>
+      </c>
+      <c r="C17" s="4" t="inlineStr">
+        <is>
+          <t>@bomboncito127</t>
+        </is>
+      </c>
+      <c r="D17" s="4" t="inlineStr">
+        <is>
+          <t>41%</t>
+        </is>
+      </c>
+      <c r="E17" s="4" t="inlineStr">
+        <is>
+          <t>Health knowledge questions</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="7" t="inlineStr">
+        <is>
+          <t>QUESTION</t>
+        </is>
+      </c>
+      <c r="B18" s="4" t="inlineStr">
+        <is>
+          <t>Question Opening</t>
+        </is>
+      </c>
+      <c r="C18" s="4" t="inlineStr">
+        <is>
+          <t>@ayunonutricion</t>
+        </is>
+      </c>
+      <c r="D18" s="4" t="inlineStr">
+        <is>
+          <t>13%</t>
+        </is>
+      </c>
+      <c r="E18" s="4" t="inlineStr">
+        <is>
+          <t>Thought-provoking questions</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="8" t="inlineStr">
+        <is>
+          <t>COMMAND</t>
+        </is>
+      </c>
+      <c r="B19" s="4" t="inlineStr">
+        <is>
+          <t>Direct Confrontation</t>
+        </is>
+      </c>
+      <c r="C19" s="4" t="inlineStr">
+        <is>
+          <t>@realmrchicago</t>
+        </is>
+      </c>
+      <c r="D19" s="4" t="inlineStr">
+        <is>
+          <t>75%</t>
+        </is>
+      </c>
+      <c r="E19" s="4" t="inlineStr">
+        <is>
+          <t>Provocative/confrontational</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="8" t="inlineStr">
+        <is>
+          <t>COMMAND</t>
+        </is>
+      </c>
+      <c r="B20" s="4" t="inlineStr">
+        <is>
+          <t>Imperative Command</t>
+        </is>
+      </c>
+      <c r="C20" s="4" t="inlineStr">
+        <is>
+          <t>@realmrchicago</t>
+        </is>
+      </c>
+      <c r="D20" s="4" t="inlineStr">
+        <is>
+          <t>13%</t>
+        </is>
+      </c>
+      <c r="E20" s="4" t="inlineStr">
+        <is>
+          <t>Direct commands</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="8" t="inlineStr">
+        <is>
+          <t>COMMAND</t>
+        </is>
+      </c>
+      <c r="B21" s="4" t="inlineStr">
+        <is>
+          <t>Attention Command</t>
+        </is>
+      </c>
+      <c r="C21" s="4" t="inlineStr">
+        <is>
+          <t>@bomboncito127</t>
+        </is>
+      </c>
+      <c r="D21" s="4" t="inlineStr">
+        <is>
+          <t>15%</t>
+        </is>
+      </c>
+      <c r="E21" s="4" t="inlineStr">
+        <is>
+          <t>"Listen to this", "Pay attention"</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="9" t="inlineStr">
+        <is>
+          <t>GREETING</t>
+        </is>
+      </c>
+      <c r="B22" s="4" t="inlineStr">
+        <is>
+          <t>Direct Greeting</t>
+        </is>
+      </c>
+      <c r="C22" s="4" t="inlineStr">
+        <is>
+          <t>@daisycabral_</t>
+        </is>
+      </c>
+      <c r="D22" s="4" t="inlineStr">
+        <is>
+          <t>75%</t>
+        </is>
+      </c>
+      <c r="E22" s="4" t="inlineStr">
+        <is>
+          <t>OUTLIER - Warm personal greeting (livestream style)</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="18" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="45" customWidth="1" min="3" max="3"/>
+    <col width="18" customWidth="1" min="4" max="4"/>
+    <col width="8" customWidth="1" min="5" max="5"/>
+    <col width="55" customWidth="1" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Semantic Category</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Reach</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Affiliates Using</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Top Performer</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Top %</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Definition</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="inlineStr">
+        <is>
+          <t>PROBLEM/PAIN</t>
+        </is>
+      </c>
+      <c r="B2" s="10" t="inlineStr">
+        <is>
+          <t>5/7 (71%)</t>
+        </is>
+      </c>
+      <c r="C2" s="4" t="inlineStr">
+        <is>
+          <t>kalimuscle, shopbyjake, ayuno, bomboncito, mrchicago</t>
+        </is>
+      </c>
+      <c r="D2" s="4" t="inlineStr">
+        <is>
+          <t>@shopbyjake</t>
+        </is>
+      </c>
+      <c r="E2" s="4" t="inlineStr">
+        <is>
+          <t>63%</t>
+        </is>
+      </c>
+      <c r="F2" s="4" t="inlineStr">
+        <is>
+          <t>Opens by identifying viewer problems, symptoms, or product issues</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="inlineStr">
+        <is>
+          <t>PRODUCT-FIRST</t>
+        </is>
+      </c>
+      <c r="B3" s="10" t="inlineStr">
+        <is>
+          <t>4/7 (57%)</t>
+        </is>
+      </c>
+      <c r="C3" s="4" t="inlineStr">
+        <is>
+          <t>yaina, ayuno, kalimuscle, daisy</t>
+        </is>
+      </c>
+      <c r="D3" s="4" t="inlineStr">
+        <is>
+          <t>@yainafashion</t>
+        </is>
+      </c>
+      <c r="E3" s="4" t="inlineStr">
+        <is>
+          <t>95%</t>
+        </is>
+      </c>
+      <c r="F3" s="4" t="inlineStr">
+        <is>
+          <t>Opens by immediately showing or presenting the product</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="6" t="inlineStr">
+        <is>
+          <t>PERSONAL/STORY</t>
+        </is>
+      </c>
+      <c r="B4" s="10" t="inlineStr">
+        <is>
+          <t>4/7 (57%)</t>
+        </is>
+      </c>
+      <c r="C4" s="4" t="inlineStr">
+        <is>
+          <t>shopbyjake, ayuno, yaina, bomboncito</t>
+        </is>
+      </c>
+      <c r="D4" s="4" t="inlineStr">
+        <is>
+          <t>@bomboncito127</t>
+        </is>
+      </c>
+      <c r="E4" s="4" t="inlineStr">
+        <is>
+          <t>20%</t>
+        </is>
+      </c>
+      <c r="F4" s="4" t="inlineStr">
+        <is>
+          <t>Opens with personal narrative, testimony, or transformation</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="7" t="inlineStr">
+        <is>
+          <t>QUESTION</t>
+        </is>
+      </c>
+      <c r="B5" s="10" t="inlineStr">
+        <is>
+          <t>3/7 (43%)</t>
+        </is>
+      </c>
+      <c r="C5" s="4" t="inlineStr">
+        <is>
+          <t>daisy, bomboncito, ayuno</t>
+        </is>
+      </c>
+      <c r="D5" s="4" t="inlineStr">
+        <is>
+          <t>@bomboncito127</t>
+        </is>
+      </c>
+      <c r="E5" s="4" t="inlineStr">
+        <is>
+          <t>41%</t>
+        </is>
+      </c>
+      <c r="F5" s="4" t="inlineStr">
+        <is>
+          <t>Opens with a thought-provoking question</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="8" t="inlineStr">
+        <is>
+          <t>COMMAND</t>
+        </is>
+      </c>
+      <c r="B6" s="10" t="inlineStr">
+        <is>
+          <t>2/7 (29%)</t>
+        </is>
+      </c>
+      <c r="C6" s="4" t="inlineStr">
+        <is>
+          <t>mrchicago, bomboncito</t>
+        </is>
+      </c>
+      <c r="D6" s="4" t="inlineStr">
+        <is>
+          <t>@realmrchicago</t>
+        </is>
+      </c>
+      <c r="E6" s="4" t="inlineStr">
+        <is>
+          <t>75%</t>
+        </is>
+      </c>
+      <c r="F6" s="4" t="inlineStr">
+        <is>
+          <t>Opens with direct commands or confrontational statements</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="9" t="inlineStr">
+        <is>
+          <t>GREETING</t>
+        </is>
+      </c>
+      <c r="B7" s="10" t="inlineStr">
+        <is>
+          <t>1/7 (14%)</t>
+        </is>
+      </c>
+      <c r="C7" s="4" t="inlineStr">
+        <is>
+          <t>daisy (OUTLIER)</t>
+        </is>
+      </c>
+      <c r="D7" s="4" t="inlineStr">
+        <is>
+          <t>@daisycabral_</t>
+        </is>
+      </c>
+      <c r="E7" s="4" t="inlineStr">
+        <is>
+          <t>75%</t>
+        </is>
+      </c>
+      <c r="F7" s="4" t="inlineStr">
+        <is>
+          <t>Opens with warm personal greeting (livestream-specific)</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="18" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
+    <col width="15" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
+    <col width="22" customWidth="1" min="8" max="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="30" customHeight="1">
+      <c r="A1" s="11" t="inlineStr">
+        <is>
+          <t>Affiliate</t>
+        </is>
+      </c>
+      <c r="B1" s="11" t="inlineStr">
+        <is>
+          <t>PROBLEM/PAIN</t>
+        </is>
+      </c>
+      <c r="C1" s="11" t="inlineStr">
+        <is>
+          <t>PRODUCT-FIRST</t>
+        </is>
+      </c>
+      <c r="D1" s="11" t="inlineStr">
+        <is>
+          <t>PERSONAL/STORY</t>
+        </is>
+      </c>
+      <c r="E1" s="11" t="inlineStr">
+        <is>
+          <t>QUESTION</t>
+        </is>
+      </c>
+      <c r="F1" s="11" t="inlineStr">
+        <is>
+          <t>COMMAND</t>
+        </is>
+      </c>
+      <c r="G1" s="11" t="inlineStr">
+        <is>
+          <t>GREETING</t>
+        </is>
+      </c>
+      <c r="H1" s="11" t="inlineStr">
+        <is>
+          <t>Dominant Hook</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="10" t="inlineStr">
+        <is>
+          <t>@daisycabral_</t>
+        </is>
+      </c>
+      <c r="B2" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C2" s="10" t="inlineStr">
+        <is>
+          <t>19%</t>
+        </is>
+      </c>
+      <c r="D2" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E2" s="10" t="inlineStr">
+        <is>
+          <t>4%</t>
+        </is>
+      </c>
+      <c r="F2" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G2" s="6" t="inlineStr">
+        <is>
+          <t>75%</t>
+        </is>
+      </c>
+      <c r="H2" s="10" t="inlineStr">
+        <is>
+          <t>GREETING (75%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="10" t="inlineStr">
+        <is>
+          <t>@realkalimuscle</t>
+        </is>
+      </c>
+      <c r="B3" s="6" t="inlineStr">
+        <is>
           <t>62%</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="C3" s="12" t="inlineStr">
+        <is>
+          <t>27%</t>
+        </is>
+      </c>
+      <c r="D3" s="10" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="E3" s="10" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>38%</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>PROMOTION + PERSONAL BRAND</t>
+      <c r="F3" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G3" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H3" s="10" t="inlineStr">
+        <is>
+          <t>PROBLEM/PAIN (62%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="10" t="inlineStr">
+        <is>
+          <t>@shopbyjake</t>
+        </is>
+      </c>
+      <c r="B4" s="6" t="inlineStr">
+        <is>
+          <t>63%</t>
+        </is>
+      </c>
+      <c r="C4" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D4" s="10" t="inlineStr">
+        <is>
+          <t>16%</t>
+        </is>
+      </c>
+      <c r="E4" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F4" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G4" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H4" s="10" t="inlineStr">
+        <is>
+          <t>PROBLEM/PAIN (63%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="10" t="inlineStr">
+        <is>
+          <t>@ayunonutricion</t>
+        </is>
+      </c>
+      <c r="B5" s="10" t="inlineStr">
+        <is>
+          <t>14%</t>
+        </is>
+      </c>
+      <c r="C5" s="6" t="inlineStr">
+        <is>
+          <t>54%</t>
+        </is>
+      </c>
+      <c r="D5" s="10" t="inlineStr">
+        <is>
+          <t>19%</t>
+        </is>
+      </c>
+      <c r="E5" s="10" t="inlineStr">
+        <is>
+          <t>13%</t>
+        </is>
+      </c>
+      <c r="F5" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G5" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H5" s="10" t="inlineStr">
+        <is>
+          <t>PRODUCT-FIRST (54%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="10" t="inlineStr">
+        <is>
+          <t>@yainafashion</t>
+        </is>
+      </c>
+      <c r="B6" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C6" s="6" t="inlineStr">
+        <is>
+          <t>95%</t>
+        </is>
+      </c>
+      <c r="D6" s="10" t="inlineStr">
+        <is>
+          <t>1%</t>
+        </is>
+      </c>
+      <c r="E6" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F6" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G6" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H6" s="10" t="inlineStr">
+        <is>
+          <t>PRODUCT-FIRST (95%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="10" t="inlineStr">
+        <is>
+          <t>@bomboncito127</t>
+        </is>
+      </c>
+      <c r="B7" s="12" t="inlineStr">
+        <is>
+          <t>23%</t>
+        </is>
+      </c>
+      <c r="C7" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D7" s="12" t="inlineStr">
+        <is>
+          <t>20%</t>
+        </is>
+      </c>
+      <c r="E7" s="12" t="inlineStr">
+        <is>
+          <t>41%</t>
+        </is>
+      </c>
+      <c r="F7" s="10" t="inlineStr">
+        <is>
+          <t>15%</t>
+        </is>
+      </c>
+      <c r="G7" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H7" s="10" t="inlineStr">
+        <is>
+          <t>QUESTION (41%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="10" t="inlineStr">
+        <is>
+          <t>@realmrchicago</t>
+        </is>
+      </c>
+      <c r="B8" s="10" t="inlineStr">
+        <is>
+          <t>11%</t>
+        </is>
+      </c>
+      <c r="C8" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D8" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E8" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F8" s="6" t="inlineStr">
+        <is>
+          <t>88%</t>
+        </is>
+      </c>
+      <c r="G8" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H8" s="10" t="inlineStr">
+        <is>
+          <t>COMMAND (88%)</t>
         </is>
       </c>
     </row>

</xml_diff>